<commit_message>
2/3 of Repository test documentation
</commit_message>
<xml_diff>
--- a/test plan/Repositories - Test Scenarios and Conditions.xlsx
+++ b/test plan/Repositories - Test Scenarios and Conditions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>Class Tested</t>
   </si>
@@ -50,9 +50,6 @@
     <t>firstName="" lastName=""</t>
   </si>
   <si>
-    <t>All employees</t>
-  </si>
-  <si>
     <t>firstName="" lastName="-1"</t>
   </si>
   <si>
@@ -132,6 +129,12 @@
   </si>
   <si>
     <t>emploeyee Ruzwana A. Bashir</t>
+  </si>
+  <si>
+    <t>All employees(size 10)</t>
+  </si>
+  <si>
+    <t>emploeyee Ruzwana A.  Bashir</t>
   </si>
 </sst>
 </file>
@@ -199,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -210,9 +213,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -221,6 +221,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -507,18 +513,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="43.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18" style="2" customWidth="1"/>
     <col min="7" max="16" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -540,291 +546,321 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="5"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>27</v>
+      <c r="F10" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>10</v>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5" t="s">
+      <c r="F19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+      <c r="C22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>25</v>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="7"/>
+      <c r="B30" s="6"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
+      <c r="B31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B12:B21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B2:B11"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="C13:C18"/>
     <mergeCell ref="D16:D18"/>
@@ -833,24 +869,6 @@
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="E13:E15"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B12:B21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B2:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>